<commit_message>
Add setup.py for cx_freeze
</commit_message>
<xml_diff>
--- a/Library/DPU01_Lib Demo2.xlsx
+++ b/Library/DPU01_Lib Demo2.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="40">
   <si>
     <t>DPU01_Lib Demo2</t>
   </si>
@@ -51,6 +51,9 @@
   </si>
   <si>
     <t>OUTPUTS</t>
+  </si>
+  <si>
+    <t>FUNCTION BLOCK DESCRIPTION</t>
   </si>
   <si>
     <t>DESCRIPTION</t>
@@ -156,7 +159,7 @@
     </font>
     <font/>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill/>
     </fill>
@@ -169,6 +172,11 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="00FFFF00"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="0000FF00"/>
       </patternFill>
     </fill>
   </fills>
@@ -209,7 +217,7 @@
     </xf>
     <xf borderId="1" fillId="3" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf borderId="1" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="1" fillId="3" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="1" fillId="4" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
@@ -580,101 +588,101 @@
         <v>2</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>4</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="11" spans="1:6">
       <c r="A11" s="5" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C11" s="4" t="n"/>
       <c r="D11" s="4" t="n"/>
     </row>
     <row r="12" spans="1:6">
       <c r="A12" s="5" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C12" s="4" t="n"/>
       <c r="D12" s="4" t="n"/>
     </row>
     <row r="13" spans="1:6">
       <c r="A13" s="5" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C13" s="4" t="n"/>
       <c r="D13" s="4" t="n"/>
     </row>
     <row r="14" spans="1:6">
       <c r="A14" s="5" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C14" s="4" t="n"/>
       <c r="D14" s="4" t="n"/>
     </row>
     <row r="15" spans="1:6">
       <c r="A15" s="5" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C15" s="4" t="n"/>
       <c r="D15" s="4" t="n"/>
     </row>
     <row r="16" spans="1:6">
       <c r="A16" s="5" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C16" s="4" t="n"/>
       <c r="D16" s="4" t="n"/>
     </row>
     <row r="17" spans="1:6">
       <c r="A17" s="5" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C17" s="4" t="n"/>
       <c r="D17" s="4" t="n"/>
     </row>
     <row r="18" spans="1:6">
       <c r="A18" s="5" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C18" s="4" t="n"/>
       <c r="D18" s="4" t="n"/>
     </row>
     <row r="19" spans="1:6">
       <c r="A19" s="5" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C19" s="4" t="n"/>
       <c r="D19" s="4" t="n"/>
@@ -682,7 +690,7 @@
     <row r="20" spans="1:6"/>
     <row r="21" spans="1:6">
       <c r="A21" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="22" spans="1:6">
@@ -696,21 +704,21 @@
         <v>4</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="F22" s="3" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="23" spans="1:6">
       <c r="A23" s="5" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C23" s="4" t="n"/>
       <c r="D23" s="4" t="n"/>
@@ -719,10 +727,10 @@
     </row>
     <row r="24" spans="1:6">
       <c r="A24" s="5" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C24" s="4" t="n"/>
       <c r="D24" s="4" t="n"/>
@@ -731,10 +739,10 @@
     </row>
     <row r="25" spans="1:6">
       <c r="A25" s="5" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C25" s="4" t="n"/>
       <c r="D25" s="4" t="n"/>

</xml_diff>